<commit_message>
Fixed some logic errors
</commit_message>
<xml_diff>
--- a/GrabFilesFromStorageBucket/test/12_10_2020.xlsx
+++ b/GrabFilesFromStorageBucket/test/12_10_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ckat\Documents\UiPath\P2Main\Team1EmptyString-P2\GrabFilesFromStorageBucket\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AFA13F-4F7F-4D95-966A-D54A75C6E177}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDEE322-938E-4201-A3F2-027B74797730}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13110" yWindow="810" windowWidth="14550" windowHeight="10740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13455" yWindow="1155" windowWidth="14550" windowHeight="10740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -31,12 +31,6 @@
     <t>Time Spent</t>
   </si>
   <si>
-    <t>00:25:00</t>
-  </si>
-  <si>
-    <t>00:30:00</t>
-  </si>
-  <si>
     <t>Zoom</t>
   </si>
   <si>
@@ -49,10 +43,16 @@
     <t>Notepad</t>
   </si>
   <si>
-    <t>06:01:16</t>
-  </si>
-  <si>
-    <t>00:08:45</t>
+    <t>00:28:00</t>
+  </si>
+  <si>
+    <t>00:10:00</t>
+  </si>
+  <si>
+    <t>06:21:16</t>
+  </si>
+  <si>
+    <t>00:03:45</t>
   </si>
 </sst>
 </file>
@@ -417,32 +417,32 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>44176</v>
+        <v>44175</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>44176</v>
+        <v>44175</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>44176</v>
+        <v>44175</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
@@ -450,10 +450,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>44176</v>
+        <v>44175</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>

</xml_diff>